<commit_message>
slight update to sprint 1 estimate + screenshots
</commit_message>
<xml_diff>
--- a/docs/group_12_sprint_1_estimate.xlsx
+++ b/docs/group_12_sprint_1_estimate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\OICE_16_974FA576_32C1D314_2B9F\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2C2F0C8-7329-4E66-AC92-CA74C777673C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{256C4088-8729-41C7-ADA8-CA55D3D51D02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="84">
   <si>
     <t>Task Name: (Dependencies top to bottom)</t>
   </si>
@@ -167,38 +167,13 @@
     <t>Architect</t>
   </si>
   <si>
-    <r>
-      <t>David</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>, Casey</t>
-    </r>
-  </si>
-  <si>
     <t>Test Report</t>
   </si>
   <si>
     <t>Tester</t>
   </si>
   <si>
-    <r>
-      <t>Casey</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>, David</t>
-    </r>
+    <t>Elias, Ibrahim, Aidan</t>
   </si>
   <si>
     <t>User Guide &amp; System Admin Doc</t>
@@ -1624,8 +1599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22:O32"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -2448,7 +2423,7 @@
         <v>37</v>
       </c>
       <c r="E18" s="49" t="s">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="F18" s="43">
         <v>6</v>
@@ -2490,13 +2465,13 @@
       <c r="A19" s="32"/>
       <c r="B19" s="32"/>
       <c r="C19" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="48" t="s">
+      <c r="E19" s="49" t="s">
         <v>40</v>
-      </c>
-      <c r="E19" s="49" t="s">
-        <v>41</v>
       </c>
       <c r="F19" s="43">
         <v>10</v>
@@ -2538,10 +2513,10 @@
       <c r="A20" s="50"/>
       <c r="B20" s="50"/>
       <c r="C20" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="52" t="s">
         <v>42</v>
-      </c>
-      <c r="D20" s="52" t="s">
-        <v>43</v>
       </c>
       <c r="E20" s="53" t="s">
         <v>35</v>
@@ -2566,10 +2541,10 @@
     </row>
     <row r="21" spans="1:32">
       <c r="A21" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="87" t="s">
         <v>44</v>
-      </c>
-      <c r="B21" s="87" t="s">
-        <v>45</v>
       </c>
       <c r="C21" s="88"/>
       <c r="D21" s="83"/>
@@ -2598,14 +2573,14 @@
     </row>
     <row r="22" spans="1:32" s="1" customFormat="1">
       <c r="A22" s="58" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B22" s="74"/>
       <c r="C22" s="66" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="67" t="s">
         <v>47</v>
-      </c>
-      <c r="D22" s="67" t="s">
-        <v>48</v>
       </c>
       <c r="E22" s="68" t="s">
         <v>28</v>
@@ -2649,7 +2624,7 @@
     <row r="23" spans="1:32" s="1" customFormat="1">
       <c r="A23" s="58"/>
       <c r="B23" s="33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" s="59"/>
       <c r="D23" s="60"/>
@@ -2695,13 +2670,13 @@
       <c r="A24" s="58"/>
       <c r="B24" s="65"/>
       <c r="C24" s="66" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="67" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="68" t="s">
         <v>50</v>
-      </c>
-      <c r="D24" s="67" t="s">
-        <v>48</v>
-      </c>
-      <c r="E24" s="68" t="s">
-        <v>51</v>
       </c>
       <c r="F24" s="69">
         <v>2</v>
@@ -2728,13 +2703,13 @@
       <c r="A25" s="58"/>
       <c r="B25" s="65"/>
       <c r="C25" s="66" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="67" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="68" t="s">
         <v>52</v>
-      </c>
-      <c r="D25" s="67" t="s">
-        <v>48</v>
-      </c>
-      <c r="E25" s="68" t="s">
-        <v>53</v>
       </c>
       <c r="F25" s="69">
         <v>12</v>
@@ -2758,13 +2733,13 @@
       <c r="A26" s="58"/>
       <c r="B26" s="65"/>
       <c r="C26" s="66" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D26" s="67" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E26" s="68" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F26" s="69">
         <v>4</v>
@@ -2788,13 +2763,13 @@
       <c r="A27" s="58"/>
       <c r="B27" s="65"/>
       <c r="C27" s="73" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D27" s="67" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E27" s="68" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F27" s="69">
         <v>10</v>
@@ -2818,13 +2793,13 @@
       <c r="A28" s="58"/>
       <c r="B28" s="74"/>
       <c r="C28" s="73" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D28" s="67" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E28" s="68" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F28" s="69">
         <v>12</v>
@@ -2848,13 +2823,13 @@
       <c r="A29" s="58"/>
       <c r="B29" s="74"/>
       <c r="C29" s="66" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D29" s="67" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E29" s="68" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F29" s="69">
         <v>4</v>
@@ -2878,13 +2853,13 @@
       <c r="A30" s="58"/>
       <c r="B30" s="74"/>
       <c r="C30" s="66" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="D30" s="67" t="s">
-        <v>48</v>
-      </c>
       <c r="E30" s="68" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F30" s="69">
         <v>2</v>
@@ -2911,7 +2886,7 @@
         <v>25</v>
       </c>
       <c r="D31" s="67" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E31" s="68" t="s">
         <v>4</v>
@@ -2932,10 +2907,10 @@
       <c r="A32" s="58"/>
       <c r="B32" s="75"/>
       <c r="C32" s="76" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D32" s="77" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E32" s="68" t="s">
         <v>4</v>
@@ -2961,7 +2936,7 @@
     <row r="33" spans="1:32">
       <c r="A33" s="58"/>
       <c r="B33" s="81" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C33" s="82"/>
       <c r="D33" s="83"/>
@@ -2989,10 +2964,10 @@
       <c r="A34" s="58"/>
       <c r="B34" s="74"/>
       <c r="C34" s="66" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D34" s="67" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E34" s="68" t="s">
         <v>22</v>
@@ -3019,10 +2994,10 @@
       <c r="A35" s="58"/>
       <c r="B35" s="74"/>
       <c r="C35" s="66" t="s">
+        <v>61</v>
+      </c>
+      <c r="D35" s="67" t="s">
         <v>62</v>
-      </c>
-      <c r="D35" s="67" t="s">
-        <v>63</v>
       </c>
       <c r="E35" s="67" t="s">
         <v>35</v>
@@ -3049,7 +3024,7 @@
       <c r="A36" s="58"/>
       <c r="B36" s="74"/>
       <c r="C36" s="66" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D36" s="67" t="s">
         <v>18</v>
@@ -3095,10 +3070,10 @@
     </row>
     <row r="37" spans="1:32">
       <c r="A37" s="86" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B37" s="87" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C37" s="88"/>
       <c r="D37" s="83"/>
@@ -3129,7 +3104,7 @@
       <c r="A38" s="86"/>
       <c r="B38" s="92"/>
       <c r="C38" s="93" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D38" s="94" t="s">
         <v>18</v>
@@ -3159,7 +3134,7 @@
       <c r="A39" s="86"/>
       <c r="B39" s="92"/>
       <c r="C39" s="93" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D39" s="94" t="s">
         <v>18</v>
@@ -3189,10 +3164,10 @@
       <c r="A40" s="86"/>
       <c r="B40" s="92"/>
       <c r="C40" s="93" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D40" s="94" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E40" s="94" t="s">
         <v>28</v>
@@ -3219,10 +3194,10 @@
       <c r="A41" s="86"/>
       <c r="B41" s="92"/>
       <c r="C41" s="93" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D41" s="94" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E41" s="95" t="s">
         <v>28</v>
@@ -3270,7 +3245,7 @@
     <row r="43" spans="1:32">
       <c r="A43" s="86"/>
       <c r="B43" s="87" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C43" s="88"/>
       <c r="D43" s="83"/>
@@ -3298,13 +3273,13 @@
       <c r="A44" s="86"/>
       <c r="B44" s="92"/>
       <c r="C44" s="93" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D44" s="94" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E44" s="95" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F44" s="96">
         <v>2</v>
@@ -3328,10 +3303,10 @@
       <c r="A45" s="86"/>
       <c r="B45" s="92"/>
       <c r="C45" s="93" t="s">
+        <v>70</v>
+      </c>
+      <c r="D45" s="94" t="s">
         <v>71</v>
-      </c>
-      <c r="D45" s="94" t="s">
-        <v>72</v>
       </c>
       <c r="E45" s="95" t="s">
         <v>3</v>
@@ -3358,13 +3333,13 @@
       <c r="A46" s="86"/>
       <c r="B46" s="92"/>
       <c r="C46" s="93" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D46" s="94" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E46" s="95" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F46" s="96">
         <v>5</v>
@@ -3388,13 +3363,13 @@
       <c r="A47" s="86"/>
       <c r="B47" s="92"/>
       <c r="C47" s="93" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D47" s="94" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E47" s="94" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F47" s="96">
         <v>6</v>
@@ -3418,13 +3393,13 @@
       <c r="A48" s="86"/>
       <c r="B48" s="92"/>
       <c r="C48" s="93" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D48" s="94" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E48" s="95" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F48" s="96">
         <v>3</v>
@@ -3451,7 +3426,7 @@
         <v>25</v>
       </c>
       <c r="D49" s="94" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E49" s="95" t="s">
         <v>4</v>
@@ -3472,10 +3447,10 @@
       <c r="A50" s="86"/>
       <c r="B50" s="99"/>
       <c r="C50" s="100" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D50" s="101" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E50" s="95" t="s">
         <v>4</v>
@@ -3501,7 +3476,7 @@
     <row r="51" spans="1:32">
       <c r="A51" s="86"/>
       <c r="B51" s="87" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C51" s="88"/>
       <c r="D51" s="83"/>
@@ -3529,10 +3504,10 @@
       <c r="A52" s="86"/>
       <c r="B52" s="92"/>
       <c r="C52" s="93" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D52" s="94" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E52" s="95" t="s">
         <v>22</v>
@@ -3559,10 +3534,10 @@
       <c r="A53" s="86"/>
       <c r="B53" s="92"/>
       <c r="C53" s="93" t="s">
+        <v>61</v>
+      </c>
+      <c r="D53" s="94" t="s">
         <v>62</v>
-      </c>
-      <c r="D53" s="94" t="s">
-        <v>63</v>
       </c>
       <c r="E53" s="106" t="s">
         <v>35</v>
@@ -3589,7 +3564,7 @@
       <c r="A54" s="86"/>
       <c r="B54" s="99"/>
       <c r="C54" s="100" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D54" s="101" t="s">
         <v>18</v>
@@ -3635,10 +3610,10 @@
     </row>
     <row r="55" spans="1:32">
       <c r="A55" s="58" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B55" s="87" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C55" s="88"/>
       <c r="D55" s="83"/>
@@ -3669,7 +3644,7 @@
       <c r="A56" s="108"/>
       <c r="B56" s="109"/>
       <c r="C56" s="110" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D56" s="111" t="s">
         <v>18</v>
@@ -3699,7 +3674,7 @@
       <c r="A57" s="58"/>
       <c r="B57" s="74"/>
       <c r="C57" s="73" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D57" s="67" t="s">
         <v>18</v>
@@ -3729,13 +3704,13 @@
       <c r="A58" s="58"/>
       <c r="B58" s="74"/>
       <c r="C58" s="73" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D58" s="67" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E58" s="119" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F58" s="118">
         <v>3</v>
@@ -3759,7 +3734,7 @@
       <c r="A59" s="58"/>
       <c r="B59" s="75"/>
       <c r="C59" s="120" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D59" s="77" t="s">
         <v>18</v>
@@ -3788,7 +3763,7 @@
     <row r="60" spans="1:32">
       <c r="A60" s="58"/>
       <c r="B60" s="87" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C60" s="88"/>
       <c r="D60" s="83"/>
@@ -3816,13 +3791,13 @@
       <c r="A61" s="58"/>
       <c r="B61" s="74"/>
       <c r="C61" s="73" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D61" s="67" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E61" s="119" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F61" s="118">
         <v>2</v>
@@ -3846,13 +3821,13 @@
       <c r="A62" s="58"/>
       <c r="B62" s="74"/>
       <c r="C62" s="73" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D62" s="67" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E62" s="119" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F62" s="118">
         <v>10</v>
@@ -3876,13 +3851,13 @@
       <c r="A63" s="58"/>
       <c r="B63" s="74"/>
       <c r="C63" s="73" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D63" s="67" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E63" s="119" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F63" s="118">
         <v>5</v>
@@ -3906,10 +3881,10 @@
       <c r="A64" s="58"/>
       <c r="B64" s="74"/>
       <c r="C64" s="73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D64" s="67" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E64" s="119" t="s">
         <v>4</v>
@@ -3936,10 +3911,10 @@
       <c r="A65" s="58"/>
       <c r="B65" s="75"/>
       <c r="C65" s="120" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D65" s="77" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E65" s="121" t="s">
         <v>4</v>
@@ -3965,7 +3940,7 @@
     <row r="66" spans="1:17">
       <c r="A66" s="58"/>
       <c r="B66" s="124" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C66" s="125"/>
       <c r="D66" s="126"/>
@@ -3993,10 +3968,10 @@
       <c r="A67" s="108"/>
       <c r="B67" s="109"/>
       <c r="C67" s="110" t="s">
+        <v>82</v>
+      </c>
+      <c r="D67" s="111" t="s">
         <v>83</v>
-      </c>
-      <c r="D67" s="111" t="s">
-        <v>84</v>
       </c>
       <c r="E67" s="131" t="s">
         <v>22</v>
@@ -4023,10 +3998,10 @@
       <c r="A68" s="133"/>
       <c r="B68" s="75"/>
       <c r="C68" s="120" t="s">
+        <v>61</v>
+      </c>
+      <c r="D68" s="77" t="s">
         <v>62</v>
-      </c>
-      <c r="D68" s="77" t="s">
-        <v>63</v>
       </c>
       <c r="E68" s="134" t="s">
         <v>35</v>

</xml_diff>